<commit_message>
Added Tron user input tab
</commit_message>
<xml_diff>
--- a/Journey/JourneyIOinputControls this might be WRONG!.xlsx
+++ b/Journey/JourneyIOinputControls this might be WRONG!.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCAdmin.SIERRA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCAdmin.SIERRA\Desktop\Franklin\ArcadeVideoGameHacking.git\Journey\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13215" windowHeight="10410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13215" windowHeight="10410" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Journey" sheetId="1" r:id="rId1"/>
+    <sheet name="Tron" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Bit</t>
   </si>
@@ -63,6 +64,36 @@
   </si>
   <si>
     <t>Port</t>
+  </si>
+  <si>
+    <t>1 Spinner</t>
+  </si>
+  <si>
+    <t>2 Spinner</t>
+  </si>
+  <si>
+    <t>1P</t>
+  </si>
+  <si>
+    <t>2P</t>
+  </si>
+  <si>
+    <t>COIN 1/L</t>
+  </si>
+  <si>
+    <t>COIN 2/R</t>
+  </si>
+  <si>
+    <t>Tilt</t>
+  </si>
+  <si>
+    <t>Service Switch</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Note: all bits are 1 (on) and flip to 0 (off or zero) when the control is activated (grounded)!</t>
   </si>
 </sst>
 </file>
@@ -70,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0000"/>
+    <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -109,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,8 +155,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,7 +442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -625,4 +659,291 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C7:I7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>